<commit_message>
SVM ya hecho con las predicciones
</commit_message>
<xml_diff>
--- a/Proyecto 1/prediccionesRandomForest.xlsx
+++ b/Proyecto 1/prediccionesRandomForest.xlsx
@@ -1007,7 +1007,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -2257,7 +2257,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -4107,7 +4107,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -4157,7 +4157,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -4257,7 +4257,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -4957,7 +4957,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -6232,7 +6232,7 @@
         </is>
       </c>
       <c r="E232" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
@@ -6832,7 +6832,7 @@
         </is>
       </c>
       <c r="E256" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257">
@@ -7007,7 +7007,7 @@
         </is>
       </c>
       <c r="E263" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="264">
@@ -8334,7 +8334,7 @@
         </is>
       </c>
       <c r="E316" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317">
@@ -8584,7 +8584,7 @@
         </is>
       </c>
       <c r="E326" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="327">
@@ -10442,7 +10442,7 @@
         </is>
       </c>
       <c r="E400" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="401">
@@ -10717,7 +10717,7 @@
         </is>
       </c>
       <c r="E411" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412">
@@ -11542,7 +11542,7 @@
         </is>
       </c>
       <c r="E444" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="445">
@@ -13867,7 +13867,7 @@
         </is>
       </c>
       <c r="E537" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="538">
@@ -14694,7 +14694,7 @@
         </is>
       </c>
       <c r="E570" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="571">
@@ -16094,7 +16094,7 @@
         </is>
       </c>
       <c r="E626" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="627">
@@ -16144,7 +16144,7 @@
         </is>
       </c>
       <c r="E628" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="629">
@@ -16869,7 +16869,7 @@
         </is>
       </c>
       <c r="E657" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="658">
@@ -20369,7 +20369,7 @@
         </is>
       </c>
       <c r="E797" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="798">
@@ -20619,7 +20619,7 @@
         </is>
       </c>
       <c r="E807" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="808">
@@ -22044,7 +22044,7 @@
         </is>
       </c>
       <c r="E864" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="865">
@@ -22369,7 +22369,7 @@
         </is>
       </c>
       <c r="E877" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="878">
@@ -23044,7 +23044,7 @@
         </is>
       </c>
       <c r="E904" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="905">

</xml_diff>

<commit_message>
Cambio Random Forest Y regresion logistica
</commit_message>
<xml_diff>
--- a/Proyecto 1/prediccionesRandomForest.xlsx
+++ b/Proyecto 1/prediccionesRandomForest.xlsx
@@ -4957,7 +4957,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -9559,7 +9559,7 @@
         </is>
       </c>
       <c r="E365" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="366">
@@ -11542,7 +11542,7 @@
         </is>
       </c>
       <c r="E444" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445">
@@ -12917,7 +12917,7 @@
         </is>
       </c>
       <c r="E499" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="500">
@@ -14694,7 +14694,7 @@
         </is>
       </c>
       <c r="E570" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="571">
@@ -16094,7 +16094,7 @@
         </is>
       </c>
       <c r="E626" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="627">
@@ -20619,7 +20619,7 @@
         </is>
       </c>
       <c r="E807" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="808">
@@ -23044,7 +23044,7 @@
         </is>
       </c>
       <c r="E904" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="905">

</xml_diff>